<commit_message>
feat: Add Total row and summary columns
</commit_message>
<xml_diff>
--- a/notebooks/samples/m_a_2025.xlsx
+++ b/notebooks/samples/m_a_2025.xlsx
@@ -656,12 +656,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -678,12 +678,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -810,12 +810,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -832,12 +832,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -964,12 +964,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -986,12 +986,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1118,12 +1118,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1140,12 +1140,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1272,12 +1272,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1294,12 +1294,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1426,12 +1426,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1448,12 +1448,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1580,12 +1580,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1602,12 +1602,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1734,12 +1734,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1756,12 +1756,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -1888,12 +1888,12 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -1910,12 +1910,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2042,12 +2042,12 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2064,12 +2064,12 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2196,12 +2196,12 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2218,12 +2218,12 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2350,12 +2350,12 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2372,12 +2372,12 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2504,12 +2504,12 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2526,12 +2526,12 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2658,12 +2658,12 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -2680,12 +2680,12 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -2812,12 +2812,12 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -2834,12 +2834,12 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -2966,12 +2966,12 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -2988,12 +2988,12 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3120,12 +3120,12 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -3142,12 +3142,12 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -3274,12 +3274,12 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -3296,12 +3296,12 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -3428,12 +3428,12 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -3450,12 +3450,12 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -3582,12 +3582,12 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -3604,12 +3604,12 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -3736,12 +3736,12 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -3758,12 +3758,12 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -3890,12 +3890,12 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -3912,12 +3912,12 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -4044,12 +4044,12 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
@@ -4066,12 +4066,12 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
@@ -4198,12 +4198,12 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
@@ -4220,12 +4220,12 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
@@ -4352,12 +4352,12 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
@@ -4374,12 +4374,12 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
@@ -4506,12 +4506,12 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
@@ -4528,12 +4528,12 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
@@ -4660,12 +4660,12 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
@@ -4682,12 +4682,12 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
@@ -4814,12 +4814,12 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
@@ -4836,12 +4836,12 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
@@ -4968,12 +4968,12 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D207" t="inlineStr">
@@ -4990,12 +4990,12 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D208" t="inlineStr">
@@ -5122,12 +5122,12 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D214" t="inlineStr">
@@ -5144,12 +5144,12 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D215" t="inlineStr">
@@ -5276,12 +5276,12 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D221" t="inlineStr">
@@ -5298,12 +5298,12 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D222" t="inlineStr">
@@ -5430,12 +5430,12 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D228" t="inlineStr">
@@ -5452,12 +5452,12 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D229" t="inlineStr">
@@ -5584,12 +5584,12 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D235" t="inlineStr">
@@ -5606,12 +5606,12 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D236" t="inlineStr">
@@ -5738,12 +5738,12 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
@@ -5760,12 +5760,12 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D243" t="inlineStr">
@@ -5892,12 +5892,12 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D249" t="inlineStr">
@@ -5914,12 +5914,12 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D250" t="inlineStr">
@@ -6046,12 +6046,12 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D256" t="inlineStr">
@@ -6068,12 +6068,12 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D257" t="inlineStr">
@@ -6200,12 +6200,12 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D263" t="inlineStr">
@@ -6222,12 +6222,12 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D264" t="inlineStr">
@@ -6354,12 +6354,12 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D270" t="inlineStr">
@@ -6376,12 +6376,12 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D271" t="inlineStr">
@@ -6508,12 +6508,12 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D277" t="inlineStr">
@@ -6530,12 +6530,12 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D278" t="inlineStr">
@@ -6662,12 +6662,12 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D284" t="inlineStr">
@@ -6684,12 +6684,12 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D285" t="inlineStr">
@@ -6816,12 +6816,12 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D291" t="inlineStr">
@@ -6838,12 +6838,12 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D292" t="inlineStr">
@@ -6970,12 +6970,12 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D298" t="inlineStr">
@@ -6992,12 +6992,12 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D299" t="inlineStr">
@@ -7124,12 +7124,12 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D305" t="inlineStr">
@@ -7146,12 +7146,12 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D306" t="inlineStr">
@@ -7278,12 +7278,12 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D312" t="inlineStr">
@@ -7300,12 +7300,12 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D313" t="inlineStr">
@@ -7432,12 +7432,12 @@
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D319" t="inlineStr">
@@ -7454,12 +7454,12 @@
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D320" t="inlineStr">
@@ -7586,12 +7586,12 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D326" t="inlineStr">
@@ -7608,12 +7608,12 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D327" t="inlineStr">
@@ -7740,12 +7740,12 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D333" t="inlineStr">
@@ -7762,12 +7762,12 @@
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D334" t="inlineStr">
@@ -7894,12 +7894,12 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D340" t="inlineStr">
@@ -7916,12 +7916,12 @@
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D341" t="inlineStr">
@@ -8048,12 +8048,12 @@
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D347" t="inlineStr">
@@ -8070,12 +8070,12 @@
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D348" t="inlineStr">
@@ -8202,12 +8202,12 @@
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D354" t="inlineStr">
@@ -8224,12 +8224,12 @@
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D355" t="inlineStr">
@@ -8356,12 +8356,12 @@
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D361" t="inlineStr">
@@ -8378,12 +8378,12 @@
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C362" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D362" t="inlineStr">
@@ -8449,7 +8449,7 @@
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D365" t="inlineStr">

</xml_diff>